<commit_message>
Initialized itself in the project.
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagai\Desktop\GitBook2.0.Net\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="19065" windowHeight="8670"/>
   </bookViews>
@@ -1315,17 +1320,17 @@
     <t>2nd</t>
   </si>
   <si>
-    <t>3rd</t>
-  </si>
-  <si>
     <t>4th</t>
+  </si>
+  <si>
+    <t>Alexey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1826,24 +1831,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -1871,6 +1876,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1917,7 +1930,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1949,9 +1962,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1983,6 +1997,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -2158,16 +2173,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DO4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:119">
+    <row r="1" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>431</v>
       </c>
@@ -2487,7 +2505,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:119">
+    <row r="2" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>432</v>
       </c>
@@ -2846,9 +2864,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:119">
+    <row r="3" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>430</v>
@@ -3169,9 +3187,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="1:119">
+    <row r="4" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B4" t="s">
         <v>327</v>

</xml_diff>